<commit_message>
Update Seguimiento de proyectos.xlsx
</commit_message>
<xml_diff>
--- a/documentacion/Seguimiento de proyectos.xlsx
+++ b/documentacion/Seguimiento de proyectos.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t>Proyecto 1</t>
   </si>
@@ -139,12 +139,6 @@
     <t>Base de datos Vacia</t>
   </si>
   <si>
-    <t xml:space="preserve">Desarrollo de procedimientos almacenados </t>
-  </si>
-  <si>
-    <t>Desarrollo de transacciones y disparadores necesarios</t>
-  </si>
-  <si>
     <t xml:space="preserve">Configuración de conexión a base de datos desde laravel </t>
   </si>
   <si>
@@ -173,12 +167,6 @@
   </si>
   <si>
     <t>Maquetado inicial del sitio mediante plantillas blade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pruebas de base de datos y conexión </t>
-  </si>
-  <si>
-    <t>Pruebas de procedimientos almacenados, transacciones y disparadores</t>
   </si>
   <si>
     <t xml:space="preserve">Configuracion de rutas según el maquetado inicial </t>
@@ -315,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +330,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -597,7 +591,7 @@
     <xf numFmtId="3" fontId="11" fillId="5" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1277,8 +1271,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SeguimientoDeProyectos" displayName="SeguimientoDeProyectos" ref="B4:O31" totalsRowShown="0" headerRowDxfId="20" tableBorderDxfId="19">
-  <autoFilter ref="B4:O31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SeguimientoDeProyectos" displayName="SeguimientoDeProyectos" ref="B4:O27" totalsRowShown="0" headerRowDxfId="20" tableBorderDxfId="19">
+  <autoFilter ref="B4:O27">
     <filterColumn colId="1">
       <filters>
         <filter val="Categoría 2"/>
@@ -1557,11 +1551,11 @@
     <tabColor theme="9"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1659,11 +1653,11 @@
       </c>
       <c r="E5" s="9">
         <f ca="1">TODAY()-65</f>
-        <v>43649</v>
+        <v>43653</v>
       </c>
       <c r="F5" s="9">
         <f ca="1">TODAY()-5</f>
-        <v>43709</v>
+        <v>43713</v>
       </c>
       <c r="G5" s="10">
         <v>210</v>
@@ -1674,11 +1668,11 @@
       </c>
       <c r="I5" s="12">
         <f ca="1">TODAY()-65</f>
-        <v>43649</v>
+        <v>43653</v>
       </c>
       <c r="J5" s="9">
         <f ca="1">TODAY()</f>
-        <v>43714</v>
+        <v>43718</v>
       </c>
       <c r="K5" s="13">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
@@ -1698,8 +1692,9 @@
       <c r="O5" s="8"/>
     </row>
     <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="41"/>
       <c r="B6" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>28</v>
@@ -1722,11 +1717,11 @@
       </c>
       <c r="I6" s="12">
         <f ca="1">TODAY()-41</f>
-        <v>43673</v>
+        <v>43677</v>
       </c>
       <c r="J6" s="9">
         <f ca="1">TODAY()-7</f>
-        <v>43707</v>
+        <v>43711</v>
       </c>
       <c r="K6" s="13">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
@@ -1757,11 +1752,11 @@
       </c>
       <c r="E7" s="9">
         <f ca="1">TODAY()-100</f>
-        <v>43614</v>
+        <v>43618</v>
       </c>
       <c r="F7" s="9">
         <f ca="1">TODAY()-40</f>
-        <v>43674</v>
+        <v>43678</v>
       </c>
       <c r="G7" s="10">
         <v>500</v>
@@ -1772,11 +1767,11 @@
       </c>
       <c r="I7" s="12">
         <f ca="1">TODAY()-100</f>
-        <v>43614</v>
+        <v>43618</v>
       </c>
       <c r="J7" s="9">
         <f ca="1">TODAY()-27</f>
-        <v>43687</v>
+        <v>43691</v>
       </c>
       <c r="K7" s="13">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
@@ -1791,13 +1786,14 @@
       </c>
       <c r="N7" s="14">
         <f ca="1">IF(COUNTA('Seguimiento de proyectos'!$I7,'Seguimiento de proyectos'!$J7)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I7,'Seguimiento de proyectos'!$J7,FALSE))</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O7" s="8"/>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="41"/>
       <c r="B8" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>28</v>
@@ -1820,11 +1816,11 @@
       </c>
       <c r="I8" s="12">
         <f ca="1">TODAY()-41</f>
-        <v>43673</v>
+        <v>43677</v>
       </c>
       <c r="J8" s="9">
         <f ca="1">TODAY()-7</f>
-        <v>43707</v>
+        <v>43711</v>
       </c>
       <c r="K8" s="13">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
@@ -1844,8 +1840,9 @@
       <c r="O8" s="8"/>
     </row>
     <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="41"/>
       <c r="B9" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>28</v>
@@ -1868,11 +1865,11 @@
       </c>
       <c r="I9" s="12">
         <f ca="1">TODAY()-41</f>
-        <v>43673</v>
+        <v>43677</v>
       </c>
       <c r="J9" s="9">
         <f ca="1">TODAY()-7</f>
-        <v>43707</v>
+        <v>43711</v>
       </c>
       <c r="K9" s="13">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
@@ -1892,6 +1889,7 @@
       <c r="O9" s="8"/>
     </row>
     <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="41"/>
       <c r="B10" s="8" t="s">
         <v>34</v>
       </c>
@@ -1915,11 +1913,11 @@
       </c>
       <c r="I10" s="12">
         <f ca="1">TODAY()-90</f>
-        <v>43624</v>
+        <v>43628</v>
       </c>
       <c r="J10" s="9">
         <f ca="1">TODAY()-71</f>
-        <v>43643</v>
+        <v>43647</v>
       </c>
       <c r="K10" s="13">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
@@ -1950,11 +1948,11 @@
       </c>
       <c r="E11" s="9">
         <f ca="1">TODAY()-90</f>
-        <v>43624</v>
+        <v>43628</v>
       </c>
       <c r="F11" s="9">
         <f ca="1">TODAY()-50</f>
-        <v>43664</v>
+        <v>43668</v>
       </c>
       <c r="G11" s="10">
         <v>300</v>
@@ -1965,11 +1963,11 @@
       </c>
       <c r="I11" s="12">
         <f ca="1">TODAY()-90</f>
-        <v>43624</v>
+        <v>43628</v>
       </c>
       <c r="J11" s="9">
         <f ca="1">TODAY()-44</f>
-        <v>43670</v>
+        <v>43674</v>
       </c>
       <c r="K11" s="13">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
@@ -2000,32 +1998,32 @@
         <v>25</v>
       </c>
       <c r="E12" s="9">
-        <v>43714</v>
+        <v>43716</v>
       </c>
       <c r="F12" s="9">
-        <v>43715</v>
+        <v>43718</v>
       </c>
       <c r="G12" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H12" s="11">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E12,'Seguimiento de proyectos'!$F12)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E12,'Seguimiento de proyectos'!$F12,FALSE))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="12">
-        <f ca="1">TODAY()-60</f>
-        <v>43654</v>
+        <f ca="1">TODAY()-45</f>
+        <v>43673</v>
       </c>
       <c r="J12" s="9">
-        <f ca="1">TODAY()-45</f>
-        <v>43669</v>
+        <f ca="1">TODAY()-5</f>
+        <v>43713</v>
       </c>
       <c r="K12" s="13">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v>1</v>
       </c>
       <c r="L12" s="10">
-        <v>510</v>
+        <v>430</v>
       </c>
       <c r="M12" s="13">
         <f ca="1">IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
@@ -2033,7 +2031,7 @@
       </c>
       <c r="N12" s="14">
         <f ca="1">IF(COUNTA('Seguimiento de proyectos'!$I12,'Seguimiento de proyectos'!$J12)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I12,'Seguimiento de proyectos'!$J12,FALSE))</f>
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="O12" s="8"/>
     </row>
@@ -2048,40 +2046,38 @@
         <v>25</v>
       </c>
       <c r="E13" s="9">
-        <v>43714</v>
+        <v>43716</v>
       </c>
       <c r="F13" s="9">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="G13" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H13" s="11">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E13,'Seguimiento de proyectos'!$F13)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E13,'Seguimiento de proyectos'!$F13,FALSE))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I13" s="12">
-        <f ca="1">TODAY()-44</f>
-        <v>43670</v>
+        <v>42434</v>
       </c>
       <c r="J13" s="9">
-        <f ca="1">TODAY()-15</f>
-        <v>43699</v>
+        <v>42495</v>
       </c>
       <c r="K13" s="13">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v>1</v>
       </c>
       <c r="L13" s="10">
-        <v>790</v>
+        <v>200</v>
       </c>
       <c r="M13" s="13">
-        <f ca="1">IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v>1</v>
       </c>
       <c r="N13" s="14">
-        <f ca="1">IF(COUNTA('Seguimiento de proyectos'!$I13,'Seguimiento de proyectos'!$J13)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I13,'Seguimiento de proyectos'!$J13,FALSE))</f>
-        <v>28</v>
+        <f>IF(COUNTA('Seguimiento de proyectos'!$I13,'Seguimiento de proyectos'!$J13)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I13,'Seguimiento de proyectos'!$J13,FALSE))</f>
+        <v>60</v>
       </c>
       <c r="O13" s="8"/>
     </row>
@@ -2096,44 +2092,36 @@
         <v>25</v>
       </c>
       <c r="E14" s="9">
-        <v>43716</v>
+        <v>43721</v>
       </c>
       <c r="F14" s="9">
-        <v>43718</v>
+        <v>43725</v>
       </c>
       <c r="G14" s="10">
         <v>5</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E14,'Seguimiento de proyectos'!$F14)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E14,'Seguimiento de proyectos'!$F14,FALSE))</f>
-        <v>2</v>
-      </c>
-      <c r="I14" s="12">
-        <f ca="1">TODAY()-45</f>
-        <v>43669</v>
-      </c>
-      <c r="J14" s="9">
-        <f ca="1">TODAY()-5</f>
-        <v>43709</v>
-      </c>
-      <c r="K14" s="13">
+        <v>4</v>
+      </c>
+      <c r="I14" s="27"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="28" t="str">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v>1</v>
-      </c>
-      <c r="L14" s="10">
-        <v>430</v>
-      </c>
-      <c r="M14" s="13">
-        <f ca="1">IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v>1</v>
-      </c>
-      <c r="N14" s="14">
-        <f ca="1">IF(COUNTA('Seguimiento de proyectos'!$I14,'Seguimiento de proyectos'!$J14)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I14,'Seguimiento de proyectos'!$J14,FALSE))</f>
-        <v>38</v>
+        <v/>
+      </c>
+      <c r="L14" s="10"/>
+      <c r="M14" s="28" t="str">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v/>
+      </c>
+      <c r="N14" s="14" t="str">
+        <f>IF(COUNTA('Seguimiento de proyectos'!$I14,'Seguimiento de proyectos'!$J14)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I14,'Seguimiento de proyectos'!$J14,FALSE))</f>
+        <v/>
       </c>
       <c r="O14" s="8"/>
     </row>
-    <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
         <v>38</v>
       </c>
@@ -2144,38 +2132,32 @@
         <v>25</v>
       </c>
       <c r="E15" s="9">
-        <v>43716</v>
+        <v>43723</v>
       </c>
       <c r="F15" s="9">
-        <v>43720</v>
+        <v>43725</v>
       </c>
       <c r="G15" s="10">
         <v>5</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E15,'Seguimiento de proyectos'!$F15)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E15,'Seguimiento de proyectos'!$F15,FALSE))</f>
-        <v>4</v>
-      </c>
-      <c r="I15" s="12">
-        <v>42434</v>
-      </c>
-      <c r="J15" s="9">
-        <v>42495</v>
-      </c>
-      <c r="K15" s="13">
+        <v>2</v>
+      </c>
+      <c r="I15" s="27"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="28" t="str">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v>1</v>
-      </c>
-      <c r="L15" s="10">
-        <v>200</v>
-      </c>
-      <c r="M15" s="13">
+        <v/>
+      </c>
+      <c r="L15" s="10"/>
+      <c r="M15" s="28" t="str">
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v>1</v>
-      </c>
-      <c r="N15" s="14">
+        <v/>
+      </c>
+      <c r="N15" s="14" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I15,'Seguimiento de proyectos'!$J15)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I15,'Seguimiento de proyectos'!$J15,FALSE))</f>
-        <v>60</v>
+        <v/>
       </c>
       <c r="O15" s="8"/>
     </row>
@@ -2190,13 +2172,13 @@
         <v>25</v>
       </c>
       <c r="E16" s="9">
-        <v>43721</v>
+        <v>43726</v>
       </c>
       <c r="F16" s="9">
-        <v>43725</v>
+        <v>43730</v>
       </c>
       <c r="G16" s="10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H16" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E16,'Seguimiento de proyectos'!$F16)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E16,'Seguimiento de proyectos'!$F16,FALSE))</f>
@@ -2219,7 +2201,8 @@
       </c>
       <c r="O16" s="8"/>
     </row>
-    <row r="17" spans="2:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="41"/>
       <c r="B17" s="8" t="s">
         <v>40</v>
       </c>
@@ -2227,20 +2210,20 @@
         <v>29</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E17" s="9">
-        <v>43723</v>
+        <v>43714</v>
       </c>
       <c r="F17" s="9">
-        <v>43725</v>
+        <v>43715</v>
       </c>
       <c r="G17" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H17" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E17,'Seguimiento de proyectos'!$F17)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E17,'Seguimiento de proyectos'!$F17,FALSE))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17" s="27"/>
       <c r="J17" s="9"/>
@@ -2259,7 +2242,8 @@
       </c>
       <c r="O17" s="8"/>
     </row>
-    <row r="18" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="41"/>
       <c r="B18" s="8" t="s">
         <v>41</v>
       </c>
@@ -2267,20 +2251,20 @@
         <v>29</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E18" s="9">
-        <v>43726</v>
+        <v>43715</v>
       </c>
       <c r="F18" s="9">
-        <v>43730</v>
+        <v>43718</v>
       </c>
       <c r="G18" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H18" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E18,'Seguimiento de proyectos'!$F18)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E18,'Seguimiento de proyectos'!$F18,FALSE))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I18" s="27"/>
       <c r="J18" s="9"/>
@@ -2299,9 +2283,9 @@
       </c>
       <c r="O18" s="8"/>
     </row>
-    <row r="19" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>29</v>
@@ -2310,17 +2294,17 @@
         <v>27</v>
       </c>
       <c r="E19" s="9">
-        <v>43714</v>
+        <v>43715</v>
       </c>
       <c r="F19" s="9">
-        <v>43715</v>
+        <v>43721</v>
       </c>
       <c r="G19" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H19" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E19,'Seguimiento de proyectos'!$F19)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E19,'Seguimiento de proyectos'!$F19,FALSE))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I19" s="27"/>
       <c r="J19" s="9"/>
@@ -2339,9 +2323,9 @@
       </c>
       <c r="O19" s="8"/>
     </row>
-    <row r="20" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>29</v>
@@ -2350,17 +2334,17 @@
         <v>27</v>
       </c>
       <c r="E20" s="9">
-        <v>43715</v>
+        <v>43719</v>
       </c>
       <c r="F20" s="9">
-        <v>43718</v>
+        <v>43721</v>
       </c>
       <c r="G20" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H20" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E20,'Seguimiento de proyectos'!$F20)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E20,'Seguimiento de proyectos'!$F20,FALSE))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I20" s="27"/>
       <c r="J20" s="9"/>
@@ -2379,7 +2363,7 @@
       </c>
       <c r="O20" s="8"/>
     </row>
-    <row r="21" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
         <v>43</v>
       </c>
@@ -2390,13 +2374,13 @@
         <v>27</v>
       </c>
       <c r="E21" s="9">
-        <v>43715</v>
+        <v>43722</v>
       </c>
       <c r="F21" s="9">
-        <v>43718</v>
+        <v>43725</v>
       </c>
       <c r="G21" s="10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H21" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E21,'Seguimiento de proyectos'!$F21)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E21,'Seguimiento de proyectos'!$F21,FALSE))</f>
@@ -2419,7 +2403,7 @@
       </c>
       <c r="O21" s="8"/>
     </row>
-    <row r="22" spans="2:15" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
         <v>44</v>
       </c>
@@ -2430,17 +2414,17 @@
         <v>27</v>
       </c>
       <c r="E22" s="9">
-        <v>43719</v>
+        <v>43726</v>
       </c>
       <c r="F22" s="9">
-        <v>43721</v>
+        <v>43729</v>
       </c>
       <c r="G22" s="10">
         <v>6</v>
       </c>
       <c r="H22" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E22,'Seguimiento de proyectos'!$F22)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E22,'Seguimiento de proyectos'!$F22,FALSE))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I22" s="27"/>
       <c r="J22" s="9"/>
@@ -2459,15 +2443,15 @@
       </c>
       <c r="O22" s="8"/>
     </row>
-    <row r="23" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23" s="9">
         <v>43722</v>
@@ -2476,7 +2460,7 @@
         <v>43725</v>
       </c>
       <c r="G23" s="10">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H23" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E23,'Seguimiento de proyectos'!$F23)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E23,'Seguimiento de proyectos'!$F23,FALSE))</f>
@@ -2499,309 +2483,149 @@
       </c>
       <c r="O23" s="8"/>
     </row>
-    <row r="24" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="9">
-        <v>43726</v>
-      </c>
-      <c r="F24" s="9">
-        <v>43729</v>
-      </c>
-      <c r="G24" s="10">
-        <v>6</v>
-      </c>
-      <c r="H24" s="26">
+    <row r="24" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="34">
+        <v>43718</v>
+      </c>
+      <c r="F24" s="34">
+        <v>43719</v>
+      </c>
+      <c r="G24" s="35">
+        <v>1</v>
+      </c>
+      <c r="H24" s="36">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E24,'Seguimiento de proyectos'!$F24)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E24,'Seguimiento de proyectos'!$F24,FALSE))</f>
-        <v>3</v>
-      </c>
-      <c r="I24" s="27"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="28" t="str">
+        <v>1</v>
+      </c>
+      <c r="I24" s="37"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="39" t="str">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="L24" s="10"/>
-      <c r="M24" s="28" t="str">
+      <c r="L24" s="35"/>
+      <c r="M24" s="39" t="str">
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="N24" s="14" t="str">
+      <c r="N24" s="40" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I24,'Seguimiento de proyectos'!$J24)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I24,'Seguimiento de proyectos'!$J24,FALSE))</f>
         <v/>
       </c>
-      <c r="O24" s="8"/>
-    </row>
-    <row r="25" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="9">
-        <v>43718</v>
-      </c>
-      <c r="F25" s="9">
-        <v>43719</v>
-      </c>
-      <c r="G25" s="10">
-        <v>4</v>
-      </c>
-      <c r="H25" s="26">
+      <c r="O24" s="33"/>
+    </row>
+    <row r="25" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="34">
+        <v>43725</v>
+      </c>
+      <c r="F25" s="34">
+        <v>43725</v>
+      </c>
+      <c r="G25" s="35">
+        <v>1</v>
+      </c>
+      <c r="H25" s="36">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E25,'Seguimiento de proyectos'!$F25)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E25,'Seguimiento de proyectos'!$F25,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="39" t="str">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v/>
+      </c>
+      <c r="L25" s="35"/>
+      <c r="M25" s="39" t="str">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v/>
+      </c>
+      <c r="N25" s="40" t="str">
+        <f>IF(COUNTA('Seguimiento de proyectos'!$I25,'Seguimiento de proyectos'!$J25)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I25,'Seguimiento de proyectos'!$J25,FALSE))</f>
+        <v/>
+      </c>
+      <c r="O25" s="33"/>
+    </row>
+    <row r="26" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="34">
+        <v>43732</v>
+      </c>
+      <c r="F26" s="34">
+        <v>43732</v>
+      </c>
+      <c r="G26" s="35">
         <v>1</v>
       </c>
-      <c r="I25" s="27"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="28" t="str">
+      <c r="H26" s="36">
+        <f>IF(COUNTA('Seguimiento de proyectos'!$E26,'Seguimiento de proyectos'!$F26)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E26,'Seguimiento de proyectos'!$F26,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="37"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="39" t="str">
         <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="L25" s="10"/>
-      <c r="M25" s="28" t="str">
+      <c r="L26" s="35"/>
+      <c r="M26" s="39" t="str">
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="N25" s="14" t="str">
-        <f>IF(COUNTA('Seguimiento de proyectos'!$I25,'Seguimiento de proyectos'!$J25)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I25,'Seguimiento de proyectos'!$J25,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O25" s="8"/>
-    </row>
-    <row r="26" spans="2:15" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="9">
-        <v>43720</v>
-      </c>
-      <c r="F26" s="9">
-        <v>43722</v>
-      </c>
-      <c r="G26" s="10">
-        <v>4</v>
-      </c>
-      <c r="H26" s="26">
-        <f>IF(COUNTA('Seguimiento de proyectos'!$E26,'Seguimiento de proyectos'!$F26)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E26,'Seguimiento de proyectos'!$F26,FALSE))</f>
-        <v>2</v>
-      </c>
-      <c r="I26" s="27"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="28" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L26" s="10"/>
-      <c r="M26" s="28" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="N26" s="14" t="str">
+      <c r="N26" s="40" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I26,'Seguimiento de proyectos'!$J26)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I26,'Seguimiento de proyectos'!$J26,FALSE))</f>
         <v/>
       </c>
-      <c r="O26" s="8"/>
-    </row>
-    <row r="27" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="9">
-        <v>43720</v>
-      </c>
-      <c r="F27" s="9">
-        <v>43722</v>
-      </c>
-      <c r="G27" s="10">
-        <v>4</v>
-      </c>
-      <c r="H27" s="26">
-        <f>IF(COUNTA('Seguimiento de proyectos'!$E27,'Seguimiento de proyectos'!$F27)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E27,'Seguimiento de proyectos'!$F27,FALSE))</f>
-        <v>2</v>
-      </c>
+      <c r="O26" s="33"/>
+    </row>
+    <row r="27" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="26"/>
       <c r="I27" s="27"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="28" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L27" s="10"/>
-      <c r="M27" s="28" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="N27" s="14" t="str">
-        <f>IF(COUNTA('Seguimiento de proyectos'!$I27,'Seguimiento de proyectos'!$J27)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I27,'Seguimiento de proyectos'!$J27,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O27" s="8"/>
-    </row>
-    <row r="28" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="34">
-        <v>43718</v>
-      </c>
-      <c r="F28" s="34">
-        <v>43718</v>
-      </c>
-      <c r="G28" s="35">
-        <v>1</v>
-      </c>
-      <c r="H28" s="36">
-        <f>IF(COUNTA('Seguimiento de proyectos'!$E28,'Seguimiento de proyectos'!$F28)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E28,'Seguimiento de proyectos'!$F28,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="37"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="39" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L28" s="35"/>
-      <c r="M28" s="39" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="N28" s="40" t="str">
-        <f>IF(COUNTA('Seguimiento de proyectos'!$I28,'Seguimiento de proyectos'!$J28)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I28,'Seguimiento de proyectos'!$J28,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O28" s="33"/>
-    </row>
-    <row r="29" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="34">
-        <v>43725</v>
-      </c>
-      <c r="F29" s="34">
-        <v>43725</v>
-      </c>
-      <c r="G29" s="35">
-        <v>1</v>
-      </c>
-      <c r="H29" s="36">
-        <f>IF(COUNTA('Seguimiento de proyectos'!$E29,'Seguimiento de proyectos'!$F29)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E29,'Seguimiento de proyectos'!$F29,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="37"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="39" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L29" s="35"/>
-      <c r="M29" s="39" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="N29" s="40" t="str">
-        <f>IF(COUNTA('Seguimiento de proyectos'!$I29,'Seguimiento de proyectos'!$J29)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I29,'Seguimiento de proyectos'!$J29,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O29" s="33"/>
-    </row>
-    <row r="30" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="34">
-        <v>43732</v>
-      </c>
-      <c r="F30" s="34">
-        <v>43732</v>
-      </c>
-      <c r="G30" s="35">
-        <v>1</v>
-      </c>
-      <c r="H30" s="36">
-        <f>IF(COUNTA('Seguimiento de proyectos'!$E30,'Seguimiento de proyectos'!$F30)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E30,'Seguimiento de proyectos'!$F30,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="37"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="39" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Trabajo real (en horas)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Trabajo real (en horas)]]-SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])/SeguimientoDeProyectos[[#This Row],[Trabajo estimado (en horas)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L30" s="35"/>
-      <c r="M30" s="39" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="N30" s="40" t="str">
-        <f>IF(COUNTA('Seguimiento de proyectos'!$I30,'Seguimiento de proyectos'!$J30)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I30,'Seguimiento de proyectos'!$J30,FALSE))</f>
-        <v/>
-      </c>
-      <c r="O30" s="33"/>
-    </row>
-    <row r="31" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="32"/>
-      <c r="O31" s="29"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="29"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L5:L7 L10:L28">
+  <conditionalFormatting sqref="L5:L7 L10:L24">
     <cfRule type="expression" dxfId="30" priority="22">
       <formula>(ABS((L5-G5))/G5)&gt;PorcentajeMarca</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5:N7 N10:N28">
+  <conditionalFormatting sqref="N5:N7 N10:N24">
     <cfRule type="expression" dxfId="29" priority="24">
       <formula>(ABS((N5-H5))/H5)&gt;PorcentajeMarca</formula>
     </cfRule>
@@ -2826,35 +2650,29 @@
       <formula>(ABS((N9-H9))/H9)&gt;PorcentajeMarca</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L29">
+  <conditionalFormatting sqref="L25">
     <cfRule type="expression" dxfId="24" priority="5">
-      <formula>(ABS((L29-G29))/G29)&gt;PorcentajeMarca</formula>
+      <formula>(ABS((L25-G25))/G25)&gt;PorcentajeMarca</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N29">
+  <conditionalFormatting sqref="N25">
     <cfRule type="expression" dxfId="23" priority="6">
-      <formula>(ABS((N29-H29))/H29)&gt;PorcentajeMarca</formula>
+      <formula>(ABS((N25-H25))/H25)&gt;PorcentajeMarca</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L30">
+  <conditionalFormatting sqref="L26">
     <cfRule type="expression" dxfId="22" priority="1">
-      <formula>(ABS((L30-G30))/G30)&gt;PorcentajeMarca</formula>
+      <formula>(ABS((L26-G26))/G26)&gt;PorcentajeMarca</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N30">
+  <conditionalFormatting sqref="N26">
     <cfRule type="expression" dxfId="21" priority="2">
-      <formula>(ABS((N30-H30))/H30)&gt;PorcentajeMarca</formula>
+      <formula>(ABS((N26-H26))/H26)&gt;PorcentajeMarca</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="18">
     <dataValidation allowBlank="1" showInputMessage="1" prompt="Indique los proyectos en la hoja de seguimiento de proyectos. Defina el porcentaje superior/inferior para D2. El trabajo real en horas y la duración real en días resaltarán los valores superior/inferior en negrita roja, y una bandera en K y M." sqref="A1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="El porcentaje superior o inferior personalizable usado para resaltar el trabajo real en horas y días en la tabla del proyecto que están por encima o por debajo de este número." sqref="D2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Seleccione una categoría de la lista o cree una categoría para mostrarla en esta lista desde la hoja de cálculo de configuración." sqref="C5:C30">
-      <formula1>ListaDeCategorías</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Seleccione un empleado de la lista o cree un empleado para mostrarlo en esta lista desde la hoja de cálculo de configuración." sqref="D5:D30">
-      <formula1>ListaDeEmpleados</formula1>
-    </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba en esta columna los nombres de proyecto" sqref="B4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seleccione en esta columna el nombre de categoría de la lista desplegable de cada celda. Las opciones de esta lista se definen en la hoja de configuración. Presione ALT+FLECHA ABAJO para recorrer la lista y ENTRAR para seleccionar." sqref="C4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seleccione el nombre del empleado en la lista desplegable en cada celda de esta columna. Las opciones se definen en la hoja de cálculo de configuración. Presione ALT+FLECHA ABAJO para ir a la lista y, después, presione ENTRAR para realizar una selección." sqref="D4"/>
@@ -2869,6 +2687,12 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el trabajo real del proyecto en horas. Los valores que cumplen los criterios de límite superior o inferior se resaltan en rojo y en negrita, y generan un icono de bandera en cada celda en la columna K de la izquierda." sqref="L4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la duración del proyecto real en días. Los valores que cumplen los criterios de límite superior o inferior se resaltan en rojo y en negrita, y generan un icono de bandera en cada celda en la columna M de la izquierda." sqref="N4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba en esta columna las notas para los proyectos." sqref="O4"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Seleccione una categoría de la lista o cree una categoría para mostrarla en esta lista desde la hoja de cálculo de configuración." sqref="C5:C26">
+      <formula1>ListaDeCategorías</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Seleccione un empleado de la lista o cree un empleado para mostrarlo en esta lista desde la hoja de cálculo de configuración." sqref="D5:D26">
+      <formula1>ListaDeEmpleados</formula1>
+    </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -2883,44 +2707,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="39" id="{981D7EE4-7E94-41DD-989D-38C05876B668}">
-            <x14:iconSet custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K5:K7 K10:K28</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="40" id="{136B1933-ABA4-46F0-A1B3-AE0D99AE777F}">
-            <x14:iconSet custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>M5:M7 M10:M28</xm:sqref>
-        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="15" id="{97F5C891-934E-4A6A-9794-8D9EC210A0C1}">
             <x14:iconSet custom="1">
@@ -3014,7 +2800,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>K29</xm:sqref>
+          <xm:sqref>K25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="8" id="{3C057907-9DB0-4088-8DDD-6A5CB2441A5A}">
@@ -3033,7 +2819,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>M29</xm:sqref>
+          <xm:sqref>M25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="3" id="{F082B105-73F9-4498-B284-7572D5D090A2}">
@@ -3052,7 +2838,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>K30</xm:sqref>
+          <xm:sqref>K26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="4" id="{668D7A0D-C0E7-463E-B61B-06EA09327A96}">
@@ -3071,7 +2857,45 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>M30</xm:sqref>
+          <xm:sqref>M26</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="77" id="{981D7EE4-7E94-41DD-989D-38C05876B668}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K5:K7 K10:K24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="80" id="{136B1933-ABA4-46F0-A1B3-AE0D99AE777F}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>M5:M7 M10:M24</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3116,7 +2940,7 @@
     </row>
     <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Cambio en el cronograma
</commit_message>
<xml_diff>
--- a/documentacion/Seguimiento de proyectos.xlsx
+++ b/documentacion/Seguimiento de proyectos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvarado\Documents\GitHub\Proyecto_Ivari\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\Proyecto_Ivari\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="78">
   <si>
     <t>Proyecto 1</t>
   </si>
@@ -257,6 +257,15 @@
   </si>
   <si>
     <t xml:space="preserve">Insercion de Productos a la pagina </t>
+  </si>
+  <si>
+    <t>Paginación en listaModificarProductos</t>
+  </si>
+  <si>
+    <t>Programación de RegistroUsuarioAdm</t>
+  </si>
+  <si>
+    <t>Programacion modificarUsuarioAdm</t>
   </si>
 </sst>
 </file>
@@ -736,7 +745,49 @@
     <cellStyle name="Título 2" xfId="6" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="10" builtinId="18" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1083,34 +1134,6 @@
       <font>
         <b/>
         <i val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
         <color theme="2" tint="-0.89996032593768116"/>
       </font>
       <fill>
@@ -1140,8 +1163,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium2">
     <tableStyle name="Estilo de tabla personalizado 2" pivot="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="24"/>
-      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="wholeTable" dxfId="26"/>
+      <tableStyleElement type="headerRow" dxfId="25"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1176,7 +1199,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Haga clic para ver la configuración"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1255,7 +1278,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Haga clic para ver los proyectos."/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1314,8 +1337,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SeguimientoDeProyectos" displayName="SeguimientoDeProyectos" ref="B4:M54" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="17">
-  <autoFilter ref="B4:M54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SeguimientoDeProyectos" displayName="SeguimientoDeProyectos" ref="B4:M57" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
+  <autoFilter ref="B4:M57">
     <filterColumn colId="1">
       <filters>
         <filter val="Categoría 2"/>
@@ -1325,35 +1348,35 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="1" name="Actividad" dataDxfId="16" dataCellStyle="Texto"/>
-    <tableColumn id="2" name="Categoría" dataDxfId="15" dataCellStyle="Texto"/>
-    <tableColumn id="3" name="Asignado a" dataDxfId="14" dataCellStyle="Texto"/>
-    <tableColumn id="4" name="Estimado_x000a_Inicio" dataDxfId="13" dataCellStyle="Fecha"/>
-    <tableColumn id="5" name="Estimado _x000a_Finalización" dataDxfId="12" dataCellStyle="Fecha"/>
-    <tableColumn id="6" name="Trabajo estimado (en horas)" dataDxfId="11" dataCellStyle="Números"/>
-    <tableColumn id="7" name="Duración estimada (en días)" dataDxfId="10" dataCellStyle="Duración estimada">
+    <tableColumn id="1" name="Actividad" dataDxfId="22" dataCellStyle="Texto"/>
+    <tableColumn id="2" name="Categoría" dataDxfId="21" dataCellStyle="Texto"/>
+    <tableColumn id="3" name="Asignado a" dataDxfId="20" dataCellStyle="Texto"/>
+    <tableColumn id="4" name="Estimado_x000a_Inicio" dataDxfId="19" dataCellStyle="Fecha"/>
+    <tableColumn id="5" name="Estimado _x000a_Finalización" dataDxfId="18" dataCellStyle="Fecha"/>
+    <tableColumn id="6" name="Trabajo estimado (en horas)" dataDxfId="17" dataCellStyle="Números"/>
+    <tableColumn id="7" name="Duración estimada (en días)" dataDxfId="16" dataCellStyle="Duración estimada">
       <calculatedColumnFormula>IF(COUNTA('Seguimiento de proyectos'!$E5,'Seguimiento de proyectos'!$F5)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E5,'Seguimiento de proyectos'!$F5,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Real _x000a_Inicio" dataDxfId="9" dataCellStyle="Inicio real"/>
-    <tableColumn id="9" name="Real_x000a_Finalización" dataDxfId="8" dataCellStyle="Fecha"/>
-    <tableColumn id="12" name="Icono de bandera para duración real superior o inferior (en días)" dataDxfId="7" dataCellStyle="Marca">
+    <tableColumn id="8" name="Real _x000a_Inicio" dataDxfId="15" dataCellStyle="Inicio real"/>
+    <tableColumn id="9" name="Real_x000a_Finalización" dataDxfId="14" dataCellStyle="Fecha"/>
+    <tableColumn id="12" name="Icono de bandera para duración real superior o inferior (en días)" dataDxfId="13" dataCellStyle="Marca">
       <calculatedColumnFormula>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Duración real (en días)" dataDxfId="6" dataCellStyle="Columna gris">
+    <tableColumn id="13" name="Duración real (en días)" dataDxfId="12" dataCellStyle="Columna gris">
       <calculatedColumnFormula>IF(COUNTA('Seguimiento de proyectos'!$I5,'Seguimiento de proyectos'!$J5)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I5,'Seguimiento de proyectos'!$J5,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Notas" dataDxfId="5" dataCellStyle="Texto"/>
+    <tableColumn id="14" name="Notas" dataDxfId="11" dataCellStyle="Texto"/>
   </tableColumns>
   <tableStyleInfo name="Estilo de tabla personalizado 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TablaDeCategoríasYEmpleados" displayName="TablaDeCategoríasYEmpleados" ref="B4:C10" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" tableBorderDxfId="2" headerRowCellStyle="Título 2" dataCellStyle="Texto">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TablaDeCategoríasYEmpleados" displayName="TablaDeCategoríasYEmpleados" ref="B4:C10" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8" headerRowCellStyle="Título 2" dataCellStyle="Texto">
   <autoFilter ref="B4:C10"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre de categoría" dataDxfId="1" dataCellStyle="Texto"/>
-    <tableColumn id="2" name="Nombre del empleado" dataDxfId="0" dataCellStyle="Texto"/>
+    <tableColumn id="1" name="Nombre de categoría" dataDxfId="7" dataCellStyle="Texto"/>
+    <tableColumn id="2" name="Nombre del empleado" dataDxfId="6" dataCellStyle="Texto"/>
   </tableColumns>
   <tableStyleInfo name="Estilo de tabla personalizado 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1590,11 +1613,11 @@
     <tabColor theme="9"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1684,11 +1707,11 @@
       </c>
       <c r="E5" s="9">
         <f ca="1">TODAY()-65</f>
-        <v>43688</v>
+        <v>43705</v>
       </c>
       <c r="F5" s="9">
         <f ca="1">TODAY()-5</f>
-        <v>43748</v>
+        <v>43765</v>
       </c>
       <c r="G5" s="10">
         <v>210</v>
@@ -1699,11 +1722,11 @@
       </c>
       <c r="I5" s="12">
         <f ca="1">TODAY()-65</f>
-        <v>43688</v>
+        <v>43705</v>
       </c>
       <c r="J5" s="9">
         <f ca="1">TODAY()</f>
-        <v>43753</v>
+        <v>43770</v>
       </c>
       <c r="K5" s="13">
         <f ca="1">IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
@@ -1711,7 +1734,7 @@
       </c>
       <c r="L5" s="14">
         <f ca="1">IF(COUNTA('Seguimiento de proyectos'!$I5,'Seguimiento de proyectos'!$J5)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I5,'Seguimiento de proyectos'!$J5,FALSE))</f>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M5" s="8"/>
     </row>
@@ -1769,11 +1792,11 @@
       </c>
       <c r="E7" s="9">
         <f ca="1">TODAY()-100</f>
-        <v>43653</v>
+        <v>43670</v>
       </c>
       <c r="F7" s="9">
         <f ca="1">TODAY()-40</f>
-        <v>43713</v>
+        <v>43730</v>
       </c>
       <c r="G7" s="10">
         <v>500</v>
@@ -1784,11 +1807,11 @@
       </c>
       <c r="I7" s="12">
         <f ca="1">TODAY()-100</f>
-        <v>43653</v>
+        <v>43670</v>
       </c>
       <c r="J7" s="9">
         <f ca="1">TODAY()-27</f>
-        <v>43726</v>
+        <v>43743</v>
       </c>
       <c r="K7" s="13">
         <f ca="1">IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
@@ -1937,11 +1960,11 @@
       </c>
       <c r="E11" s="9">
         <f ca="1">TODAY()-90</f>
-        <v>43663</v>
+        <v>43680</v>
       </c>
       <c r="F11" s="9">
         <f ca="1">TODAY()-50</f>
-        <v>43703</v>
+        <v>43720</v>
       </c>
       <c r="G11" s="10">
         <v>300</v>
@@ -1952,11 +1975,11 @@
       </c>
       <c r="I11" s="12">
         <f ca="1">TODAY()-90</f>
-        <v>43663</v>
+        <v>43680</v>
       </c>
       <c r="J11" s="9">
         <f ca="1">TODAY()-44</f>
-        <v>43709</v>
+        <v>43726</v>
       </c>
       <c r="K11" s="13">
         <f ca="1">IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
@@ -1964,7 +1987,7 @@
       </c>
       <c r="L11" s="14">
         <f ca="1">IF(COUNTA('Seguimiento de proyectos'!$I11,'Seguimiento de proyectos'!$J11)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I11,'Seguimiento de proyectos'!$J11,FALSE))</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M11" s="8"/>
     </row>
@@ -2576,11 +2599,13 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L26" s="48">
+      <c r="L26" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I26,'Seguimiento de proyectos'!$J26)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I26,'Seguimiento de proyectos'!$J26,FALSE))</f>
         <v>4</v>
       </c>
-      <c r="M26" s="38"/>
+      <c r="M26" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
@@ -2615,11 +2640,13 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L27" s="48">
+      <c r="L27" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I27,'Seguimiento de proyectos'!$J27)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I27,'Seguimiento de proyectos'!$J27,FALSE))</f>
         <v>3</v>
       </c>
-      <c r="M27" s="38"/>
+      <c r="M27" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="28" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="38" t="s">
@@ -2654,11 +2681,13 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L28" s="48">
+      <c r="L28" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I28,'Seguimiento de proyectos'!$J28)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I28,'Seguimiento de proyectos'!$J28,FALSE))</f>
         <v>4</v>
       </c>
-      <c r="M28" s="38"/>
+      <c r="M28" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="38" t="s">
@@ -2693,11 +2722,13 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L29" s="48">
+      <c r="L29" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I29,'Seguimiento de proyectos'!$J29)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I29,'Seguimiento de proyectos'!$J29,FALSE))</f>
         <v>3</v>
       </c>
-      <c r="M29" s="38"/>
+      <c r="M29" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="29" t="s">
@@ -2732,11 +2763,13 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L30" s="48">
+      <c r="L30" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I30,'Seguimiento de proyectos'!$J30)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I30,'Seguimiento de proyectos'!$J30,FALSE))</f>
         <v>9</v>
       </c>
-      <c r="M30" s="38"/>
+      <c r="M30" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="51" t="s">
@@ -2771,11 +2804,13 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L31" s="48">
+      <c r="L31" s="35">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I31,'Seguimiento de proyectos'!$J31)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I31,'Seguimiento de proyectos'!$J31,FALSE))</f>
         <v>3</v>
       </c>
-      <c r="M31" s="38"/>
+      <c r="M31" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="38" t="s">
@@ -2810,11 +2845,13 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L32" s="48">
+      <c r="L32" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I32,'Seguimiento de proyectos'!$J32)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I32,'Seguimiento de proyectos'!$J32,FALSE))</f>
         <v>3</v>
       </c>
-      <c r="M32" s="38"/>
+      <c r="M32" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="33" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="38" t="s">
@@ -2849,11 +2886,13 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L33" s="48">
+      <c r="L33" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I33,'Seguimiento de proyectos'!$J33)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I33,'Seguimiento de proyectos'!$J33,FALSE))</f>
         <v>5</v>
       </c>
-      <c r="M33" s="38"/>
+      <c r="M33" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="34" spans="2:13" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B34" s="38" t="s">
@@ -2888,11 +2927,13 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L34" s="48">
+      <c r="L34" s="26">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I34,'Seguimiento de proyectos'!$J34)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I34,'Seguimiento de proyectos'!$J34,FALSE))</f>
         <v>5</v>
       </c>
-      <c r="M34" s="38"/>
+      <c r="M34" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="35" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B35" s="38" t="s">
@@ -2917,15 +2958,19 @@
         <f>IF(COUNTA('Seguimiento de proyectos'!$E35,'Seguimiento de proyectos'!$F35)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E35,'Seguimiento de proyectos'!$F35,FALSE))</f>
         <v>2</v>
       </c>
-      <c r="I35" s="36"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="37" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L35" s="54" t="str">
+      <c r="I35" s="49">
+        <v>43753</v>
+      </c>
+      <c r="J35" s="49">
+        <v>43755</v>
+      </c>
+      <c r="K35" s="37">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="54">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I35,'Seguimiento de proyectos'!$J35)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I35,'Seguimiento de proyectos'!$J35,FALSE))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="M35" s="38"/>
     </row>
@@ -2952,15 +2997,19 @@
         <f>IF(COUNTA('Seguimiento de proyectos'!$E36,'Seguimiento de proyectos'!$F36)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E36,'Seguimiento de proyectos'!$F36,FALSE))</f>
         <v>3</v>
       </c>
-      <c r="I36" s="36"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="37" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L36" s="54" t="str">
+      <c r="I36" s="49">
+        <v>43753</v>
+      </c>
+      <c r="J36" s="49">
+        <v>43756</v>
+      </c>
+      <c r="K36" s="37">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="54">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I36,'Seguimiento de proyectos'!$J36)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I36,'Seguimiento de proyectos'!$J36,FALSE))</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="M36" s="38"/>
     </row>
@@ -2987,19 +3036,23 @@
         <f>IF(COUNTA('Seguimiento de proyectos'!$E37,'Seguimiento de proyectos'!$F37)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E37,'Seguimiento de proyectos'!$F37,FALSE))</f>
         <v>3</v>
       </c>
-      <c r="I37" s="36"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="37" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L37" s="54" t="str">
+      <c r="I37" s="49">
+        <v>43753</v>
+      </c>
+      <c r="J37" s="49">
+        <v>43756</v>
+      </c>
+      <c r="K37" s="37">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="54">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I37,'Seguimiento de proyectos'!$J37)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I37,'Seguimiento de proyectos'!$J37,FALSE))</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="M37" s="38"/>
     </row>
-    <row r="38" spans="2:13" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="38" t="s">
         <v>73</v>
       </c>
@@ -3022,15 +3075,19 @@
         <f>IF(COUNTA('Seguimiento de proyectos'!$E38,'Seguimiento de proyectos'!$F38)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E38,'Seguimiento de proyectos'!$F38,FALSE))</f>
         <v>3</v>
       </c>
-      <c r="I38" s="36"/>
-      <c r="J38" s="49"/>
-      <c r="K38" s="37" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L38" s="54" t="str">
+      <c r="I38" s="9">
+        <v>43757</v>
+      </c>
+      <c r="J38" s="9">
+        <v>43760</v>
+      </c>
+      <c r="K38" s="37">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="54">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I38,'Seguimiento de proyectos'!$J38)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I38,'Seguimiento de proyectos'!$J38,FALSE))</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="M38" s="38"/>
     </row>
@@ -3057,56 +3114,64 @@
         <f>IF(COUNTA('Seguimiento de proyectos'!$E39,'Seguimiento de proyectos'!$F39)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E39,'Seguimiento de proyectos'!$F39,FALSE))</f>
         <v>3</v>
       </c>
-      <c r="I39" s="36"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="37" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L39" s="48" t="str">
+      <c r="I39" s="9">
+        <v>43757</v>
+      </c>
+      <c r="J39" s="9">
+        <v>43760</v>
+      </c>
+      <c r="K39" s="37">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L39" s="54">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I39,'Seguimiento de proyectos'!$J39)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I39,'Seguimiento de proyectos'!$J39,FALSE))</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="M39" s="38"/>
     </row>
     <row r="40" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="38" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E40" s="9">
         <v>43761</v>
       </c>
       <c r="F40" s="9">
-        <v>43766</v>
+        <v>43763</v>
       </c>
       <c r="G40" s="40">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H40" s="35">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E40,'Seguimiento de proyectos'!$F40)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E40,'Seguimiento de proyectos'!$F40,FALSE))</f>
-        <v>5</v>
-      </c>
-      <c r="I40" s="36"/>
-      <c r="J40" s="39"/>
-      <c r="K40" s="37" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L40" s="54" t="str">
+        <v>2</v>
+      </c>
+      <c r="I40" s="9">
+        <v>43761</v>
+      </c>
+      <c r="J40" s="9">
+        <v>43769</v>
+      </c>
+      <c r="K40" s="37">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="L40" s="54">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I40,'Seguimiento de proyectos'!$J40)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I40,'Seguimiento de proyectos'!$J40,FALSE))</f>
-        <v/>
+        <v>8</v>
       </c>
       <c r="M40" s="38"/>
     </row>
     <row r="41" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="38" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C41" s="23" t="s">
         <v>27</v>
@@ -3127,21 +3192,25 @@
         <f>IF(COUNTA('Seguimiento de proyectos'!$E41,'Seguimiento de proyectos'!$F41)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E41,'Seguimiento de proyectos'!$F41,FALSE))</f>
         <v>2</v>
       </c>
-      <c r="I41" s="36"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="37" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L41" s="48" t="str">
+      <c r="I41" s="9">
+        <v>43761</v>
+      </c>
+      <c r="J41" s="9">
+        <v>43769</v>
+      </c>
+      <c r="K41" s="37">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="L41" s="54">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I41,'Seguimiento de proyectos'!$J41)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I41,'Seguimiento de proyectos'!$J41,FALSE))</f>
-        <v/>
+        <v>8</v>
       </c>
       <c r="M41" s="38"/>
     </row>
     <row r="42" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C42" s="23" t="s">
         <v>27</v>
@@ -3162,21 +3231,25 @@
         <f>IF(COUNTA('Seguimiento de proyectos'!$E42,'Seguimiento de proyectos'!$F42)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E42,'Seguimiento de proyectos'!$F42,FALSE))</f>
         <v>2</v>
       </c>
-      <c r="I42" s="36"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="37" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L42" s="54" t="str">
+      <c r="I42" s="9">
+        <v>43761</v>
+      </c>
+      <c r="J42" s="9">
+        <v>43769</v>
+      </c>
+      <c r="K42" s="37">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="L42" s="54">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I42,'Seguimiento de proyectos'!$J42)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I42,'Seguimiento de proyectos'!$J42,FALSE))</f>
-        <v/>
+        <v>8</v>
       </c>
       <c r="M42" s="38"/>
     </row>
     <row r="43" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="38" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C43" s="23" t="s">
         <v>27</v>
@@ -3185,10 +3258,10 @@
         <v>23</v>
       </c>
       <c r="E43" s="9">
-        <v>43761</v>
+        <v>43764</v>
       </c>
       <c r="F43" s="9">
-        <v>43763</v>
+        <v>43766</v>
       </c>
       <c r="G43" s="40">
         <v>2</v>
@@ -3197,40 +3270,44 @@
         <f>IF(COUNTA('Seguimiento de proyectos'!$E43,'Seguimiento de proyectos'!$F43)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E43,'Seguimiento de proyectos'!$F43,FALSE))</f>
         <v>2</v>
       </c>
-      <c r="I43" s="36"/>
-      <c r="J43" s="39"/>
-      <c r="K43" s="37" t="str">
-        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
-        <v/>
-      </c>
-      <c r="L43" s="48" t="str">
+      <c r="I43" s="9">
+        <v>43764</v>
+      </c>
+      <c r="J43" s="9">
+        <v>43769</v>
+      </c>
+      <c r="K43" s="37">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="L43" s="54">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I43,'Seguimiento de proyectos'!$J43)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I43,'Seguimiento de proyectos'!$J43,FALSE))</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="M43" s="38"/>
     </row>
     <row r="44" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="38" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E44" s="9">
-        <v>43764</v>
+        <v>43771</v>
       </c>
       <c r="F44" s="9">
-        <v>43766</v>
+        <v>43775</v>
       </c>
       <c r="G44" s="40">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H44" s="35">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E44,'Seguimiento de proyectos'!$F44)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E44,'Seguimiento de proyectos'!$F44,FALSE))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I44" s="36"/>
       <c r="J44" s="39"/>
@@ -3238,7 +3315,7 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="L44" s="48" t="str">
+      <c r="L44" s="54" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I44,'Seguimiento de proyectos'!$J44)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I44,'Seguimiento de proyectos'!$J44,FALSE))</f>
         <v/>
       </c>
@@ -3246,7 +3323,7 @@
     </row>
     <row r="45" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="38" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>27</v>
@@ -3255,17 +3332,17 @@
         <v>23</v>
       </c>
       <c r="E45" s="9">
-        <v>43764</v>
+        <v>43771</v>
       </c>
       <c r="F45" s="9">
-        <v>43766</v>
+        <v>43775</v>
       </c>
       <c r="G45" s="40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H45" s="35">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E45,'Seguimiento de proyectos'!$F45)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E45,'Seguimiento de proyectos'!$F45,FALSE))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I45" s="36"/>
       <c r="J45" s="39"/>
@@ -3273,7 +3350,7 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="L45" s="48" t="str">
+      <c r="L45" s="54" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I45,'Seguimiento de proyectos'!$J45)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I45,'Seguimiento de proyectos'!$J45,FALSE))</f>
         <v/>
       </c>
@@ -3281,7 +3358,7 @@
     </row>
     <row r="46" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="38" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C46" s="23" t="s">
         <v>27</v>
@@ -3290,17 +3367,17 @@
         <v>23</v>
       </c>
       <c r="E46" s="9">
-        <v>43767</v>
+        <v>43771</v>
       </c>
       <c r="F46" s="9">
-        <v>43770</v>
+        <v>43775</v>
       </c>
       <c r="G46" s="40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H46" s="35">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E46,'Seguimiento de proyectos'!$F46)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E46,'Seguimiento de proyectos'!$F46,FALSE))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I46" s="36"/>
       <c r="J46" s="39"/>
@@ -3308,15 +3385,15 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="L46" s="48" t="str">
+      <c r="L46" s="54" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I46,'Seguimiento de proyectos'!$J46)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I46,'Seguimiento de proyectos'!$J46,FALSE))</f>
         <v/>
       </c>
       <c r="M46" s="38"/>
     </row>
-    <row r="47" spans="2:13" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="38" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="C47" s="23" t="s">
         <v>27</v>
@@ -3328,14 +3405,14 @@
         <v>43771</v>
       </c>
       <c r="F47" s="9">
-        <v>43773</v>
+        <v>43775</v>
       </c>
       <c r="G47" s="40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H47" s="35">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E47,'Seguimiento de proyectos'!$F47)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E47,'Seguimiento de proyectos'!$F47,FALSE))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I47" s="36"/>
       <c r="J47" s="39"/>
@@ -3343,7 +3420,7 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="L47" s="48" t="str">
+      <c r="L47" s="54" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I47,'Seguimiento de proyectos'!$J47)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I47,'Seguimiento de proyectos'!$J47,FALSE))</f>
         <v/>
       </c>
@@ -3351,7 +3428,7 @@
     </row>
     <row r="48" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="38" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C48" s="23" t="s">
         <v>27</v>
@@ -3360,13 +3437,13 @@
         <v>23</v>
       </c>
       <c r="E48" s="9">
-        <v>43774</v>
+        <v>43764</v>
       </c>
       <c r="F48" s="9">
-        <v>43776</v>
+        <v>43766</v>
       </c>
       <c r="G48" s="40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H48" s="35">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E48,'Seguimiento de proyectos'!$F48)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E48,'Seguimiento de proyectos'!$F48,FALSE))</f>
@@ -3378,7 +3455,7 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="L48" s="48" t="str">
+      <c r="L48" s="54" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I48,'Seguimiento de proyectos'!$J48)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I48,'Seguimiento de proyectos'!$J48,FALSE))</f>
         <v/>
       </c>
@@ -3386,7 +3463,7 @@
     </row>
     <row r="49" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="38" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C49" s="23" t="s">
         <v>27</v>
@@ -3395,17 +3472,17 @@
         <v>23</v>
       </c>
       <c r="E49" s="9">
-        <v>43777</v>
+        <v>43767</v>
       </c>
       <c r="F49" s="9">
-        <v>43780</v>
+        <v>43770</v>
       </c>
       <c r="G49" s="40">
         <v>3</v>
       </c>
       <c r="H49" s="35">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E49,'Seguimiento de proyectos'!$F49)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E49,'Seguimiento de proyectos'!$F49,FALSE))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I49" s="36"/>
       <c r="J49" s="39"/>
@@ -3413,7 +3490,7 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="L49" s="48" t="str">
+      <c r="L49" s="54" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I49,'Seguimiento de proyectos'!$J49)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I49,'Seguimiento de proyectos'!$J49,FALSE))</f>
         <v/>
       </c>
@@ -3421,7 +3498,7 @@
     </row>
     <row r="50" spans="2:13" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B50" s="38" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C50" s="23" t="s">
         <v>27</v>
@@ -3430,17 +3507,17 @@
         <v>23</v>
       </c>
       <c r="E50" s="9">
-        <v>43777</v>
+        <v>43771</v>
       </c>
       <c r="F50" s="9">
-        <v>43780</v>
+        <v>43773</v>
       </c>
       <c r="G50" s="40">
         <v>3</v>
       </c>
       <c r="H50" s="35">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E50,'Seguimiento de proyectos'!$F50)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E50,'Seguimiento de proyectos'!$F50,FALSE))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I50" s="36"/>
       <c r="J50" s="39"/>
@@ -3448,22 +3525,34 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="L50" s="48" t="str">
+      <c r="L50" s="54" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I50,'Seguimiento de proyectos'!$J50)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I50,'Seguimiento de proyectos'!$J50,FALSE))</f>
         <v/>
       </c>
       <c r="M50" s="38"/>
     </row>
     <row r="51" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="38"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="49"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="35" t="str">
+      <c r="B51" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="9">
+        <v>43774</v>
+      </c>
+      <c r="F51" s="9">
+        <v>43776</v>
+      </c>
+      <c r="G51" s="40">
+        <v>2</v>
+      </c>
+      <c r="H51" s="35">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E51,'Seguimiento de proyectos'!$F51)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E51,'Seguimiento de proyectos'!$F51,FALSE))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="I51" s="36"/>
       <c r="J51" s="39"/>
@@ -3471,22 +3560,34 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="L51" s="50" t="str">
+      <c r="L51" s="54" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I51,'Seguimiento de proyectos'!$J51)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I51,'Seguimiento de proyectos'!$J51,FALSE))</f>
         <v/>
       </c>
       <c r="M51" s="38"/>
     </row>
     <row r="52" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="38"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="49"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="35" t="str">
+      <c r="B52" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="9">
+        <v>43777</v>
+      </c>
+      <c r="F52" s="9">
+        <v>43780</v>
+      </c>
+      <c r="G52" s="40">
+        <v>3</v>
+      </c>
+      <c r="H52" s="35">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E52,'Seguimiento de proyectos'!$F52)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E52,'Seguimiento de proyectos'!$F52,FALSE))</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="I52" s="36"/>
       <c r="J52" s="39"/>
@@ -3494,22 +3595,34 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="L52" s="50" t="str">
+      <c r="L52" s="54" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I52,'Seguimiento de proyectos'!$J52)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I52,'Seguimiento de proyectos'!$J52,FALSE))</f>
         <v/>
       </c>
       <c r="M52" s="38"/>
     </row>
-    <row r="53" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="38"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="49"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="35" t="str">
+    <row r="53" spans="2:13" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B53" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" s="9">
+        <v>43777</v>
+      </c>
+      <c r="F53" s="9">
+        <v>43780</v>
+      </c>
+      <c r="G53" s="40">
+        <v>3</v>
+      </c>
+      <c r="H53" s="35">
         <f>IF(COUNTA('Seguimiento de proyectos'!$E53,'Seguimiento de proyectos'!$F53)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E53,'Seguimiento de proyectos'!$F53,FALSE))</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="I53" s="36"/>
       <c r="J53" s="39"/>
@@ -3517,45 +3630,119 @@
         <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
         <v/>
       </c>
-      <c r="L53" s="50" t="str">
+      <c r="L53" s="54" t="str">
         <f>IF(COUNTA('Seguimiento de proyectos'!$I53,'Seguimiento de proyectos'!$J53)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I53,'Seguimiento de proyectos'!$J53,FALSE))</f>
         <v/>
       </c>
       <c r="M53" s="38"/>
     </row>
     <row r="54" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="51"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="52"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="53"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="27"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="28"/>
-      <c r="L54" s="32"/>
-      <c r="M54" s="29"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="35" t="str">
+        <f>IF(COUNTA('Seguimiento de proyectos'!$E54,'Seguimiento de proyectos'!$F54)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E54,'Seguimiento de proyectos'!$F54,FALSE))</f>
+        <v/>
+      </c>
+      <c r="I54" s="36"/>
+      <c r="J54" s="39"/>
+      <c r="K54" s="37" t="str">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v/>
+      </c>
+      <c r="L54" s="54" t="str">
+        <f>IF(COUNTA('Seguimiento de proyectos'!$I54,'Seguimiento de proyectos'!$J54)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I54,'Seguimiento de proyectos'!$J54,FALSE))</f>
+        <v/>
+      </c>
+      <c r="M54" s="38"/>
+    </row>
+    <row r="55" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="38"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="35" t="str">
+        <f>IF(COUNTA('Seguimiento de proyectos'!$E55,'Seguimiento de proyectos'!$F55)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E55,'Seguimiento de proyectos'!$F55,FALSE))</f>
+        <v/>
+      </c>
+      <c r="I55" s="36"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="37" t="str">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v/>
+      </c>
+      <c r="L55" s="50" t="str">
+        <f>IF(COUNTA('Seguimiento de proyectos'!$I55,'Seguimiento de proyectos'!$J55)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I55,'Seguimiento de proyectos'!$J55,FALSE))</f>
+        <v/>
+      </c>
+      <c r="M55" s="38"/>
+    </row>
+    <row r="56" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="38"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="35" t="str">
+        <f>IF(COUNTA('Seguimiento de proyectos'!$E56,'Seguimiento de proyectos'!$F56)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$E56,'Seguimiento de proyectos'!$F56,FALSE))</f>
+        <v/>
+      </c>
+      <c r="I56" s="36"/>
+      <c r="J56" s="39"/>
+      <c r="K56" s="37" t="str">
+        <f>IFERROR(IF(SeguimientoDeProyectos[Duración real (en días)]=0,"",IF(ABS((SeguimientoDeProyectos[[#This Row],[Duración real (en días)]]-SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])/SeguimientoDeProyectos[[#This Row],[Duración estimada (en días)]])&gt;PorcentajeMarca,1,0)),"")</f>
+        <v/>
+      </c>
+      <c r="L56" s="50" t="str">
+        <f>IF(COUNTA('Seguimiento de proyectos'!$I56,'Seguimiento de proyectos'!$J56)&lt;&gt;2,"",DAYS360('Seguimiento de proyectos'!$I56,'Seguimiento de proyectos'!$J56,FALSE))</f>
+        <v/>
+      </c>
+      <c r="M56" s="38"/>
+    </row>
+    <row r="57" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="51"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="51"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="52"/>
+      <c r="G57" s="53"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="30"/>
+      <c r="K57" s="28"/>
+      <c r="L57" s="32"/>
+      <c r="M57" s="29"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L10:L50">
-    <cfRule type="expression" dxfId="22" priority="25">
+  <conditionalFormatting sqref="L10:L25 L35:L47">
+    <cfRule type="expression" dxfId="4" priority="26">
       <formula>(ABS((L10-H10))/H10)&gt;PorcentajeMarca</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:L7">
-    <cfRule type="expression" dxfId="21" priority="27">
+    <cfRule type="expression" dxfId="3" priority="28">
       <formula>(ABS((L5-H5))/H5)&gt;PorcentajeMarca</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="expression" dxfId="20" priority="17">
+    <cfRule type="expression" dxfId="2" priority="18">
       <formula>(ABS((L8-H8))/H8)&gt;PorcentajeMarca</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="expression" dxfId="19" priority="13">
+    <cfRule type="expression" dxfId="1" priority="14">
       <formula>(ABS((L9-H9))/H9)&gt;PorcentajeMarca</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L48:L54">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>(ABS((L48-H48))/H48)&gt;PorcentajeMarca</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
@@ -3573,10 +3760,10 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Bandera de duración real sup./inf. (días) del título de tabla de proyectos. Los valores de N que cumplen el límite sup./inf. generan una bandera en cada celda de la columna. Las celdas en blanco indican que los valores no cumplen el límite sup./inf." sqref="K4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la duración del proyecto real en días. Los valores que cumplen los criterios de límite superior o inferior se resaltan en rojo y en negrita, y generan un icono de bandera en cada celda en la columna M de la izquierda." sqref="L4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba en esta columna las notas para los proyectos." sqref="M4"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Seleccione una categoría de la lista o cree una categoría para mostrarla en esta lista desde la hoja de cálculo de configuración." sqref="C5:C53">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Seleccione una categoría de la lista o cree una categoría para mostrarla en esta lista desde la hoja de cálculo de configuración." sqref="C5:C56">
       <formula1>ListaDeCategorías</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Seleccione un empleado de la lista o cree un empleado para mostrarlo en esta lista desde la hoja de cálculo de configuración." sqref="D5:D53">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Seleccione un empleado de la lista o cree un empleado para mostrarlo en esta lista desde la hoja de cálculo de configuración." sqref="D5:D56">
       <formula1>ListaDeEmpleados</formula1>
     </dataValidation>
   </dataValidations>
@@ -3594,7 +3781,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="19" id="{59DAD741-96EE-4524-81F3-5C74A995E026}">
+          <x14:cfRule type="iconSet" priority="20" id="{59DAD741-96EE-4524-81F3-5C74A995E026}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3613,7 +3800,7 @@
           <xm:sqref>K8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="15" id="{0CC0C0A4-7FD4-4DA1-930C-9F9BEFEFEB72}">
+          <x14:cfRule type="iconSet" priority="16" id="{0CC0C0A4-7FD4-4DA1-930C-9F9BEFEFEB72}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3632,7 +3819,7 @@
           <xm:sqref>K9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="80" id="{981D7EE4-7E94-41DD-989D-38C05876B668}">
+          <x14:cfRule type="iconSet" priority="81" id="{981D7EE4-7E94-41DD-989D-38C05876B668}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3651,7 +3838,7 @@
           <xm:sqref>K10:K24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="83" id="{136B1933-ABA4-46F0-A1B3-AE0D99AE777F}">
+          <x14:cfRule type="iconSet" priority="84" id="{136B1933-ABA4-46F0-A1B3-AE0D99AE777F}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3670,7 +3857,7 @@
           <xm:sqref>K5:K7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="89" id="{3C057907-9DB0-4088-8DDD-6A5CB2441A5A}">
+          <x14:cfRule type="iconSet" priority="90" id="{3C057907-9DB0-4088-8DDD-6A5CB2441A5A}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3686,7 +3873,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>K25:K53</xm:sqref>
+          <xm:sqref>K25:K56</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>